<commit_message>
fixed routes and refactored code
</commit_message>
<xml_diff>
--- a/public/assets/student_sample.xlsx
+++ b/public/assets/student_sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhanu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhanu\Desktop\GitHub\college-management\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D985D2B-2D14-42B7-9913-6CAF74F3B815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A6C6EC-E7EA-493A-9D64-599A7DC62792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>f_name</t>
   </si>
@@ -78,24 +78,6 @@
     <t>session_end_year</t>
   </si>
   <si>
-    <t>course_fee</t>
-  </si>
-  <si>
-    <t>exam_fee</t>
-  </si>
-  <si>
-    <t>library_fee</t>
-  </si>
-  <si>
-    <t>practical_fee</t>
-  </si>
-  <si>
-    <t>security_fee</t>
-  </si>
-  <si>
-    <t>con_fee</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
@@ -208,15 +190,6 @@
   </si>
   <si>
     <t>B. Com</t>
-  </si>
-  <si>
-    <t>bus_fee</t>
-  </si>
-  <si>
-    <t>hostel_fee</t>
-  </si>
-  <si>
-    <t>paid_fee</t>
   </si>
 </sst>
 </file>
@@ -552,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA201"/>
+  <dimension ref="A1:S201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +538,7 @@
     <col min="24" max="24" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,73 +590,46 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F2">
         <v>511</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M2">
         <v>2211</v>
@@ -692,7 +638,7 @@
         <v>23423</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="P2">
         <v>2019</v>
@@ -703,70 +649,46 @@
       <c r="R2">
         <v>45000</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>3000</v>
-      </c>
-      <c r="V2">
-        <v>4000</v>
-      </c>
-      <c r="W2">
-        <v>4000</v>
-      </c>
-      <c r="X2">
-        <v>5000</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="F3">
         <v>512</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M3">
         <v>2212</v>
@@ -775,7 +697,7 @@
         <v>23424</v>
       </c>
       <c r="O3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="P3">
         <v>2019</v>
@@ -786,70 +708,46 @@
       <c r="R3">
         <v>45000</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>3000</v>
-      </c>
-      <c r="V3">
-        <v>4000</v>
-      </c>
-      <c r="W3">
-        <v>4000</v>
-      </c>
-      <c r="X3">
-        <v>5000</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F4">
         <v>513</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M4">
         <v>2213</v>
@@ -858,7 +756,7 @@
         <v>23425</v>
       </c>
       <c r="O4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="P4">
         <v>2019</v>
@@ -869,70 +767,46 @@
       <c r="R4">
         <v>45000</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>3000</v>
-      </c>
-      <c r="V4">
-        <v>4000</v>
-      </c>
-      <c r="W4">
-        <v>4000</v>
-      </c>
-      <c r="X4">
-        <v>5000</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="F5">
         <v>514</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M5">
         <v>2214</v>
@@ -941,7 +815,7 @@
         <v>23426</v>
       </c>
       <c r="O5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="P5">
         <v>2019</v>
@@ -952,70 +826,46 @@
       <c r="R5">
         <v>45000</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>3000</v>
-      </c>
-      <c r="V5">
-        <v>4000</v>
-      </c>
-      <c r="W5">
-        <v>4000</v>
-      </c>
-      <c r="X5">
-        <v>5000</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="F6">
         <v>515</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M6">
         <v>2215</v>
@@ -1024,7 +874,7 @@
         <v>23427</v>
       </c>
       <c r="O6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="P6">
         <v>2019</v>
@@ -1035,70 +885,46 @@
       <c r="R6">
         <v>45000</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>3000</v>
-      </c>
-      <c r="V6">
-        <v>4000</v>
-      </c>
-      <c r="W6">
-        <v>4000</v>
-      </c>
-      <c r="X6">
-        <v>5000</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="F7">
         <v>516</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="M7">
         <v>2216</v>
@@ -1107,7 +933,7 @@
         <v>23428</v>
       </c>
       <c r="O7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="P7">
         <v>2019</v>
@@ -1118,59 +944,35 @@
       <c r="R7">
         <v>45000</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>3000</v>
-      </c>
-      <c r="V7">
-        <v>4000</v>
-      </c>
-      <c r="W7">
-        <v>4000</v>
-      </c>
-      <c r="X7">
-        <v>5000</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">

</xml_diff>